<commit_message>
update process export excel
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5175" yWindow="1800" windowWidth="28035" windowHeight="17445"/>
+    <workbookView xWindow="5175" yWindow="1800" windowWidth="28035" windowHeight="17445" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
     <sheet name="config" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="47">
   <si>
     <t>totalGroup</t>
   </si>
@@ -44,36 +45,6 @@
     <t>range_1</t>
   </si>
   <si>
-    <t>B2</t>
-  </si>
-  <si>
-    <t>E4</t>
-  </si>
-  <si>
-    <t>Group: &lt;#table.NAME_GROUP&gt;</t>
-  </si>
-  <si>
-    <t>End group: &lt;#table.END_GROUP&gt;</t>
-  </si>
-  <si>
-    <t>#</t>
-  </si>
-  <si>
-    <t>Mã</t>
-  </si>
-  <si>
-    <t>Tên</t>
-  </si>
-  <si>
-    <t>&lt;#table.ROW_NUM&gt;</t>
-  </si>
-  <si>
-    <t>&lt;#table.CODE&gt;</t>
-  </si>
-  <si>
-    <t>&lt;#table.NAME&gt;</t>
-  </si>
-  <si>
     <t>begin</t>
   </si>
   <si>
@@ -83,32 +54,137 @@
     <t>range_0</t>
   </si>
   <si>
-    <t>NAME_GROUP,END_GROUP</t>
-  </si>
-  <si>
     <t>PARENT</t>
   </si>
   <si>
-    <t>&lt;#table.PARENT&gt;</t>
+    <t>end line</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>ROW_NUM</t>
+  </si>
+  <si>
+    <t>CODE</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>NAME_GROUP</t>
+  </si>
+  <si>
+    <t>END_GROUP</t>
+  </si>
+  <si>
+    <t>A001</t>
+  </si>
+  <si>
+    <t>Nguyen Van A001</t>
+  </si>
+  <si>
+    <t>Group 1</t>
+  </si>
+  <si>
+    <t>Parent 1</t>
+  </si>
+  <si>
+    <t>A002</t>
+  </si>
+  <si>
+    <t>Nguyen Van A002</t>
+  </si>
+  <si>
+    <t>A003</t>
+  </si>
+  <si>
+    <t>Nguyen Van A003</t>
+  </si>
+  <si>
+    <t>A004</t>
+  </si>
+  <si>
+    <t>Nguyen Van A004</t>
+  </si>
+  <si>
+    <t>Group 2</t>
+  </si>
+  <si>
+    <t>A005</t>
+  </si>
+  <si>
+    <t>Nguyen Van A005</t>
+  </si>
+  <si>
+    <t>A006</t>
+  </si>
+  <si>
+    <t>Nguyen Van A006</t>
+  </si>
+  <si>
+    <t>Parent 2</t>
+  </si>
+  <si>
+    <t>A007</t>
+  </si>
+  <si>
+    <t>Nguyen Van A007</t>
+  </si>
+  <si>
+    <t>A008</t>
+  </si>
+  <si>
+    <t>Nguyen Van A008</t>
+  </si>
+  <si>
+    <t>A009</t>
+  </si>
+  <si>
+    <t>Nguyen Van A009</t>
+  </si>
+  <si>
+    <t>A010</t>
+  </si>
+  <si>
+    <t>Nguyen Van A010</t>
+  </si>
+  <si>
+    <t>Parent &lt;#PARENT&gt;</t>
+  </si>
+  <si>
+    <t>&lt;#NAME&gt;</t>
+  </si>
+  <si>
+    <t>&lt;#ROW_NUM&gt;</t>
+  </si>
+  <si>
+    <t>&lt;#CODE&gt;</t>
   </si>
   <si>
     <t>range_2</t>
   </si>
   <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>Group &lt;#NAME_GROUP&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
     <t>B1</t>
   </si>
   <si>
-    <t>E5</t>
-  </si>
-  <si>
-    <t>B4</t>
+    <t>C1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -122,37 +198,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.89999084444715716"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -162,7 +235,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
+        <fgColor theme="1" tint="4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF7FCCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -231,44 +316,42 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF7FCCC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -597,70 +680,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:5">
-      <c r="B1" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-    </row>
-    <row r="2" spans="2:5">
-      <c r="B2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9"/>
-    </row>
-    <row r="3" spans="2:5">
-      <c r="B3" s="10" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="8"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75">
+      <c r="A5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5">
-      <c r="B4" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5">
-      <c r="B5" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
       <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A5:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -668,13 +766,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="135.109375" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" customWidth="1"/>
     <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
@@ -683,64 +781,522 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6">
+      <c r="B1" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="B3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="5"/>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>16</v>
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>15</v>
+      <c r="B5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="6"/>
+      <c r="A6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20">
+        <v>7</v>
+      </c>
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21">
+        <v>8</v>
+      </c>
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22">
+        <v>9</v>
+      </c>
+      <c r="B22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23">
+        <v>10</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add function merge cell
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -41,6 +41,30 @@
     <author>AdonisGM</author>
   </authors>
   <commentList>
+    <comment ref="A7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>merge_id:&lt;#NAME_GROUP&gt;</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>AdonisGM</author>
+  </authors>
+  <commentList>
     <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
@@ -194,7 +218,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>totalGroup</t>
   </si>
@@ -256,26 +280,29 @@
     <t>A6</t>
   </si>
   <si>
-    <t>C7</t>
-  </si>
-  <si>
     <t>A7</t>
   </si>
   <si>
-    <t>C8</t>
-  </si>
-  <si>
     <t>End Group &lt;#NAME_GROUP&gt;</t>
   </si>
   <si>
     <t>End General: &lt;#GENERAL_NAME_REPORT&gt;</t>
+  </si>
+  <si>
+    <t>Merge Cell</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>D7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -335,6 +362,13 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -420,7 +454,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -442,6 +476,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -800,83 +837,90 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.109375" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="25.44140625" customWidth="1"/>
+    <col min="2" max="3" width="14.44140625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75">
+    <row r="3" spans="1:4" ht="15.75">
       <c r="A3" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="9"/>
+      <c r="C5" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="11" t="s">
+    <row r="6" spans="1:4">
+      <c r="A6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="12"/>
+      <c r="B6" s="13"/>
       <c r="C6" s="13"/>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="5" t="s">
+      <c r="D6" s="14"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="C7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="15"/>
+    <row r="8" spans="1:4">
+      <c r="A8" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="16"/>
       <c r="C8" s="16"/>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D8" s="17"/>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A8:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -885,7 +929,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15.75"/>
@@ -915,7 +959,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -923,7 +967,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -945,7 +989,7 @@
         <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>5</v>
@@ -956,10 +1000,10 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D7" s="1"/>
     </row>

</xml_diff>

<commit_message>
Optimize merge and process data
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -27,30 +27,6 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Nguyễn Mạnh Tùng</author>
-  </authors>
-  <commentList>
-    <comment ref="A7" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>merge_id:&lt;#merge.NAME_GROUP&gt;</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
     <author>AdonisGM</author>
   </authors>
   <commentList>
@@ -284,14 +260,14 @@
     <t>End General: &lt;#general.GENERAL_NAME_REPORT&gt;</t>
   </si>
   <si>
-    <t>&lt;#table.NAME_GROUP&gt;</t>
+    <t>&lt;#table.NAME_GROUP&gt;&lt;#merge.&lt;#table.NAME_GROUP&gt;&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -350,13 +326,6 @@
       <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -830,21 +799,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.109375" customWidth="1"/>
+    <col min="1" max="1" width="27.33203125" customWidth="1"/>
     <col min="2" max="3" width="14.44140625" style="8" customWidth="1"/>
     <col min="4" max="4" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.95">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -854,7 +823,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.95">
+    <row r="5" spans="1:4">
       <c r="A5" s="4"/>
       <c r="B5" s="9" t="s">
         <v>11</v>
@@ -866,7 +835,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.95">
+    <row r="6" spans="1:4">
       <c r="A6" s="12" t="s">
         <v>21</v>
       </c>
@@ -874,7 +843,7 @@
       <c r="C6" s="13"/>
       <c r="D6" s="14"/>
     </row>
-    <row r="7" spans="1:4" ht="15.95">
+    <row r="7" spans="1:4">
       <c r="A7" s="11" t="s">
         <v>25</v>
       </c>
@@ -888,7 +857,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.95">
+    <row r="8" spans="1:4">
       <c r="A8" s="15" t="s">
         <v>22</v>
       </c>
@@ -896,12 +865,12 @@
       <c r="C8" s="16"/>
       <c r="D8" s="17"/>
     </row>
-    <row r="10" spans="1:4" ht="15.95">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.95">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -913,7 +882,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -922,7 +890,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
Support export multiple sheet
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5175" yWindow="1800" windowWidth="28035" windowHeight="17445"/>
+    <workbookView xWindow="5175" yWindow="1800" windowWidth="28035" windowHeight="17445" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
-    <sheet name="config" sheetId="2" r:id="rId2"/>
+    <sheet name="Report (2)" sheetId="5" r:id="rId2"/>
+    <sheet name="Report (3)" sheetId="6" r:id="rId3"/>
+    <sheet name="config" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913" iterate="1"/>
   <extLst>
@@ -50,7 +52,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Tổng số bảng lồng nhau</t>
+0: Report không chưa thông tin chung
+1: Report có chứa thông tin chung</t>
         </r>
       </text>
     </comment>
@@ -74,8 +77,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-0: Report không chưa thông tin chung
-1: Report có chứa thông tin chung</t>
+0: Không có merge cell trong report
+1: Có merge cell trong report</t>
         </r>
       </text>
     </comment>
@@ -153,6 +156,154 @@
       </text>
     </comment>
     <comment ref="D5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>AdonisGM:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Các cột thông tin của bảng,
+Nếu là bảng cuối cùng không điền tên cột vì sẽ lấy all
+Nếu có nhiều cột thì ngăn cách bằng dấu ",". VD: "ABC,EDO"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>AdonisGM:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Toạ độ bắt đầu của bảng</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>AdonisGM:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Toạ độ kết thúc của bảng</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>AdonisGM:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Các cột thông tin của bảng,
+Nếu là bảng cuối cùng không điền tên cột vì sẽ lấy all
+Nếu có nhiều cột thì ngăn cách bằng dấu ",". VD: "ABC,EDO"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B13" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>AdonisGM:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Toạ độ bắt đầu của bảng</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C13" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>AdonisGM:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Toạ độ kết thúc của bảng</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -183,10 +334,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
-  <si>
-    <t>totalGroup</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="30">
   <si>
     <t>range_1</t>
   </si>
@@ -264,6 +412,18 @@
   </si>
   <si>
     <t>A8</t>
+  </si>
+  <si>
+    <t>isMultipleSheet</t>
+  </si>
+  <si>
+    <t>sheet_0</t>
+  </si>
+  <si>
+    <t>sheet_1</t>
+  </si>
+  <si>
+    <t>sheet_2</t>
   </si>
 </sst>
 </file>
@@ -415,7 +575,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -448,6 +608,27 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -466,21 +647,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -826,8 +993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="15"/>
@@ -839,37 +1006,37 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75">
       <c r="A3" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="4"/>
       <c r="B5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="D5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="16"/>
+      <c r="A6" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="23"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="20" t="s">
-        <v>24</v>
+      <c r="A7" s="16" t="s">
+        <v>23</v>
       </c>
       <c r="B7" s="5">
         <f>SUM(B8:B9)</f>
@@ -880,40 +1047,40 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="D8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="21"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="24"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="20"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="19"/>
+      <c r="A10" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="26"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -927,11 +1094,219 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="27.33203125" customWidth="1"/>
+    <col min="2" max="3" width="14.44140625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75">
+      <c r="A3" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="4"/>
+      <c r="B5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="23"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="5">
+        <f>SUM(B8:B9)</f>
+        <v>0</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="15"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="17"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="20"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="26"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A10:D10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="27.33203125" customWidth="1"/>
+    <col min="2" max="3" width="14.44140625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75">
+      <c r="A3" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="4"/>
+      <c r="B5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="23"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="5">
+        <f>SUM(B8:B9)</f>
+        <v>0</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="15"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="17"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="20"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="26"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A10:D10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="15.75"/>
@@ -950,15 +1325,15 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -966,48 +1341,131 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4">
+      <c r="A5" s="27" t="s">
+        <v>27</v>
+      </c>
       <c r="B5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>3</v>
-      </c>
       <c r="D5" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="1"/>
+      <c r="C9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>